<commit_message>
Modifs cartes + blog
</commit_message>
<xml_diff>
--- a/src/data/BDD_observation.xlsx
+++ b/src/data/BDD_observation.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jadoo\OneDrive\Documents\PROJETS\BDD guardianmap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GDM_REACT_JS\guardian_map\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08C1D40-E51C-4DED-AFE1-55D47248F0CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B01ADB5-E5B6-4A38-969D-1DE0F0EBF997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="135" windowWidth="19170" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$75</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -859,7 +862,7 @@
   <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L70" sqref="L70"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2341,6 +2344,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F75" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>